<commit_message>
Implement basic extract routines
</commit_message>
<xml_diff>
--- a/test/schedule.xlsx
+++ b/test/schedule.xlsx
@@ -736,7 +736,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4967" uniqueCount="2051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4967" uniqueCount="2053">
   <si>
     <t>Instructor</t>
   </si>
@@ -9289,6 +9289,14 @@
   <si>
     <t>대학A 229</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>스토이메노프</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GS1001-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -9946,7 +9954,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="113">
+  <borders count="111">
     <border>
       <left/>
       <right/>
@@ -11290,30 +11298,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -11419,7 +11403,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="909">
+  <cellXfs count="905">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -12338,7 +12322,7 @@
     <xf numFmtId="178" fontId="30" fillId="14" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="109" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="107" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="178" fontId="30" fillId="6" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12377,7 +12361,7 @@
     <xf numFmtId="178" fontId="30" fillId="14" borderId="54" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="110" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="108" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="53" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13647,9 +13631,6 @@
     <xf numFmtId="0" fontId="38" fillId="2" borderId="68" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="98" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="99" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -14019,10 +14000,10 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="103" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="107" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="105" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="108" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="106" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="68" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14073,7 +14054,7 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="39" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="106" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="104" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14082,10 +14063,10 @@
     <xf numFmtId="0" fontId="38" fillId="2" borderId="103" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="107" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="105" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="108" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="106" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="68" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14103,25 +14084,16 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="53" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="111" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="109" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="112" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="110" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="2" borderId="78" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="103" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="104" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="105" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="81" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -23260,23 +23232,23 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
-      <c r="N2" s="858"/>
-      <c r="O2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
+      <c r="N2" s="857"/>
+      <c r="O2" s="857"/>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:15" ht="43.5" customHeight="1" thickBot="1">
@@ -23341,7 +23313,7 @@
       <c r="F5" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G5" s="859" t="s">
+      <c r="G5" s="858" t="s">
         <v>819</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -23380,7 +23352,7 @@
       <c r="F6" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G6" s="860"/>
+      <c r="G6" s="859"/>
       <c r="H6" s="9" t="s">
         <v>387</v>
       </c>
@@ -23417,7 +23389,7 @@
       <c r="F7" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G7" s="860"/>
+      <c r="G7" s="859"/>
       <c r="H7" s="9" t="s">
         <v>387</v>
       </c>
@@ -23454,7 +23426,7 @@
       <c r="F8" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G8" s="860"/>
+      <c r="G8" s="859"/>
       <c r="H8" s="9" t="s">
         <v>387</v>
       </c>
@@ -23491,7 +23463,7 @@
       <c r="F9" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G9" s="860"/>
+      <c r="G9" s="859"/>
       <c r="H9" s="9" t="s">
         <v>387</v>
       </c>
@@ -23528,7 +23500,7 @@
       <c r="F10" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G10" s="860"/>
+      <c r="G10" s="859"/>
       <c r="H10" s="9" t="s">
         <v>387</v>
       </c>
@@ -23565,7 +23537,7 @@
       <c r="F11" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G11" s="861"/>
+      <c r="G11" s="860"/>
       <c r="H11" s="9" t="s">
         <v>387</v>
       </c>
@@ -25515,7 +25487,7 @@
       <c r="F64" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G64" s="862" t="s">
+      <c r="G64" s="861" t="s">
         <v>1104</v>
       </c>
       <c r="H64" s="9" t="s">
@@ -25554,7 +25526,7 @@
       <c r="F65" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G65" s="860"/>
+      <c r="G65" s="859"/>
       <c r="H65" s="9" t="s">
         <v>380</v>
       </c>
@@ -25591,7 +25563,7 @@
       <c r="F66" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="G66" s="861"/>
+      <c r="G66" s="860"/>
       <c r="H66" s="9" t="s">
         <v>422</v>
       </c>
@@ -30145,23 +30117,23 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="26.25">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>979</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
-      <c r="N2" s="858"/>
-      <c r="O2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
+      <c r="N2" s="857"/>
+      <c r="O2" s="857"/>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:15" ht="43.5" customHeight="1" thickBot="1">
@@ -30877,23 +30849,23 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="26.25">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>979</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
-      <c r="N2" s="858"/>
-      <c r="O2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
+      <c r="N2" s="857"/>
+      <c r="O2" s="857"/>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:15" ht="43.5" customHeight="1" thickBot="1">
@@ -31546,21 +31518,21 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="26.25">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>822</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" thickBot="1"/>
     <row r="4" spans="1:13" ht="34.5">
@@ -31603,7 +31575,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="647" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A5" s="907" t="s">
+      <c r="A5" s="903" t="s">
         <v>1062</v>
       </c>
       <c r="B5" s="642" t="s">
@@ -31636,7 +31608,7 @@
       <c r="M5" s="646"/>
     </row>
     <row r="6" spans="1:13" s="647" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A6" s="907"/>
+      <c r="A6" s="903"/>
       <c r="B6" s="642" t="s">
         <v>1144</v>
       </c>
@@ -31665,7 +31637,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="647" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A7" s="908"/>
+      <c r="A7" s="904"/>
       <c r="B7" s="650" t="s">
         <v>1145</v>
       </c>
@@ -31744,21 +31716,21 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="24.95" customHeight="1">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
     </row>
     <row r="3" spans="1:14" ht="12.95" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:14" ht="43.5" customHeight="1" thickBot="1">
@@ -31891,7 +31863,7 @@
       <c r="F7" s="176" t="s">
         <v>171</v>
       </c>
-      <c r="G7" s="863" t="s">
+      <c r="G7" s="862" t="s">
         <v>820</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -31929,7 +31901,7 @@
       <c r="F8" s="176" t="s">
         <v>171</v>
       </c>
-      <c r="G8" s="864"/>
+      <c r="G8" s="863"/>
       <c r="H8" s="9" t="s">
         <v>437</v>
       </c>
@@ -31965,7 +31937,7 @@
       <c r="F9" s="176" t="s">
         <v>171</v>
       </c>
-      <c r="G9" s="865"/>
+      <c r="G9" s="864"/>
       <c r="H9" s="9" t="s">
         <v>437</v>
       </c>
@@ -32306,14 +32278,14 @@
       <selection activeCell="F8" sqref="F8"/>
       <selection pane="topRight" activeCell="F8" sqref="F8"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
-      <selection pane="bottomRight" activeCell="AN58" sqref="AN58"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="321" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="321" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="745" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="744" customWidth="1"/>
     <col min="4" max="19" width="10.5703125" style="321" customWidth="1"/>
     <col min="20" max="75" width="10.7109375" style="321" customWidth="1"/>
     <col min="76" max="16384" width="9.140625" style="321"/>
@@ -32324,7 +32296,7 @@
         <v>2020</v>
       </c>
       <c r="B1" s="322"/>
-      <c r="C1" s="754"/>
+      <c r="C1" s="753"/>
       <c r="D1" s="322"/>
       <c r="E1" s="322"/>
       <c r="F1" s="322"/>
@@ -32401,7 +32373,7 @@
     <row r="2" spans="1:75" ht="13.5">
       <c r="A2" s="322"/>
       <c r="B2" s="322"/>
-      <c r="C2" s="754"/>
+      <c r="C2" s="753"/>
       <c r="D2" s="322"/>
       <c r="E2" s="322"/>
       <c r="F2" s="322"/>
@@ -32478,7 +32450,7 @@
     <row r="3" spans="1:75" ht="14.25" thickBot="1">
       <c r="A3" s="322"/>
       <c r="B3" s="322"/>
-      <c r="C3" s="754"/>
+      <c r="C3" s="753"/>
       <c r="D3" s="322"/>
       <c r="E3" s="322"/>
       <c r="F3" s="322"/>
@@ -32554,103 +32526,103 @@
     </row>
     <row r="4" spans="1:75" ht="18" thickBot="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="895" t="s">
+      <c r="B4" s="894" t="s">
         <v>2019</v>
       </c>
-      <c r="C4" s="896"/>
-      <c r="D4" s="899" t="s">
+      <c r="C4" s="895"/>
+      <c r="D4" s="883" t="s">
         <v>2018</v>
       </c>
-      <c r="E4" s="900"/>
-      <c r="F4" s="900"/>
-      <c r="G4" s="900"/>
-      <c r="H4" s="900"/>
-      <c r="I4" s="901"/>
-      <c r="J4" s="901"/>
-      <c r="K4" s="901"/>
-      <c r="L4" s="901"/>
-      <c r="M4" s="901"/>
-      <c r="N4" s="901"/>
-      <c r="O4" s="901"/>
-      <c r="P4" s="743"/>
-      <c r="Q4" s="743"/>
-      <c r="R4" s="743"/>
-      <c r="S4" s="743"/>
-      <c r="T4" s="903" t="s">
+      <c r="E4" s="884"/>
+      <c r="F4" s="884"/>
+      <c r="G4" s="884"/>
+      <c r="H4" s="884"/>
+      <c r="I4" s="884"/>
+      <c r="J4" s="884"/>
+      <c r="K4" s="884"/>
+      <c r="L4" s="884"/>
+      <c r="M4" s="884"/>
+      <c r="N4" s="884"/>
+      <c r="O4" s="884"/>
+      <c r="P4" s="884"/>
+      <c r="Q4" s="884"/>
+      <c r="R4" s="884"/>
+      <c r="S4" s="884"/>
+      <c r="T4" s="899" t="s">
         <v>2017</v>
       </c>
-      <c r="U4" s="903"/>
-      <c r="V4" s="903"/>
-      <c r="W4" s="903"/>
-      <c r="X4" s="903"/>
-      <c r="Y4" s="903"/>
-      <c r="Z4" s="903"/>
-      <c r="AA4" s="903"/>
-      <c r="AB4" s="903"/>
-      <c r="AC4" s="903"/>
-      <c r="AD4" s="903"/>
-      <c r="AE4" s="903"/>
-      <c r="AF4" s="903"/>
-      <c r="AG4" s="903"/>
-      <c r="AH4" s="903"/>
-      <c r="AI4" s="903"/>
-      <c r="AJ4" s="902" t="s">
+      <c r="U4" s="899"/>
+      <c r="V4" s="899"/>
+      <c r="W4" s="899"/>
+      <c r="X4" s="899"/>
+      <c r="Y4" s="899"/>
+      <c r="Z4" s="899"/>
+      <c r="AA4" s="899"/>
+      <c r="AB4" s="899"/>
+      <c r="AC4" s="899"/>
+      <c r="AD4" s="899"/>
+      <c r="AE4" s="899"/>
+      <c r="AF4" s="899"/>
+      <c r="AG4" s="899"/>
+      <c r="AH4" s="899"/>
+      <c r="AI4" s="899"/>
+      <c r="AJ4" s="898" t="s">
         <v>2016</v>
       </c>
-      <c r="AK4" s="903"/>
-      <c r="AL4" s="903"/>
-      <c r="AM4" s="903"/>
-      <c r="AN4" s="903"/>
-      <c r="AO4" s="903"/>
-      <c r="AP4" s="903"/>
-      <c r="AQ4" s="903"/>
-      <c r="AR4" s="903"/>
-      <c r="AS4" s="903"/>
-      <c r="AT4" s="903"/>
-      <c r="AU4" s="903"/>
-      <c r="AV4" s="903"/>
-      <c r="AW4" s="903"/>
-      <c r="AX4" s="903"/>
-      <c r="AY4" s="903"/>
-      <c r="AZ4" s="884" t="s">
+      <c r="AK4" s="899"/>
+      <c r="AL4" s="899"/>
+      <c r="AM4" s="899"/>
+      <c r="AN4" s="899"/>
+      <c r="AO4" s="899"/>
+      <c r="AP4" s="899"/>
+      <c r="AQ4" s="899"/>
+      <c r="AR4" s="899"/>
+      <c r="AS4" s="899"/>
+      <c r="AT4" s="899"/>
+      <c r="AU4" s="899"/>
+      <c r="AV4" s="899"/>
+      <c r="AW4" s="899"/>
+      <c r="AX4" s="899"/>
+      <c r="AY4" s="899"/>
+      <c r="AZ4" s="883" t="s">
         <v>2015</v>
       </c>
-      <c r="BA4" s="885"/>
-      <c r="BB4" s="885"/>
-      <c r="BC4" s="885"/>
-      <c r="BD4" s="885"/>
-      <c r="BE4" s="885"/>
-      <c r="BF4" s="885"/>
-      <c r="BG4" s="885"/>
-      <c r="BH4" s="885"/>
-      <c r="BI4" s="885"/>
-      <c r="BJ4" s="885"/>
-      <c r="BK4" s="885"/>
-      <c r="BL4" s="885"/>
-      <c r="BM4" s="885"/>
-      <c r="BN4" s="885"/>
-      <c r="BO4" s="885"/>
-      <c r="BP4" s="886"/>
-      <c r="BQ4" s="884" t="s">
+      <c r="BA4" s="884"/>
+      <c r="BB4" s="884"/>
+      <c r="BC4" s="884"/>
+      <c r="BD4" s="884"/>
+      <c r="BE4" s="884"/>
+      <c r="BF4" s="884"/>
+      <c r="BG4" s="884"/>
+      <c r="BH4" s="884"/>
+      <c r="BI4" s="884"/>
+      <c r="BJ4" s="884"/>
+      <c r="BK4" s="884"/>
+      <c r="BL4" s="884"/>
+      <c r="BM4" s="884"/>
+      <c r="BN4" s="884"/>
+      <c r="BO4" s="884"/>
+      <c r="BP4" s="885"/>
+      <c r="BQ4" s="883" t="s">
         <v>2014</v>
       </c>
-      <c r="BR4" s="885"/>
-      <c r="BS4" s="885"/>
-      <c r="BT4" s="885"/>
-      <c r="BU4" s="885"/>
-      <c r="BV4" s="885"/>
-      <c r="BW4" s="886"/>
+      <c r="BR4" s="884"/>
+      <c r="BS4" s="884"/>
+      <c r="BT4" s="884"/>
+      <c r="BU4" s="884"/>
+      <c r="BV4" s="884"/>
+      <c r="BW4" s="885"/>
     </row>
     <row r="5" spans="1:75" s="203" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="202"/>
-      <c r="B5" s="872" t="s">
+      <c r="B5" s="871" t="s">
         <v>2013</v>
       </c>
-      <c r="C5" s="772" t="s">
+      <c r="C5" s="771" t="s">
         <v>1311</v>
       </c>
       <c r="D5" s="207" t="s">
-        <v>1413</v>
+        <v>2052</v>
       </c>
       <c r="E5" s="223" t="s">
         <v>2012</v>
@@ -32754,7 +32726,7 @@
       <c r="BN5" s="114"/>
       <c r="BO5" s="114"/>
       <c r="BP5" s="114"/>
-      <c r="BQ5" s="834" t="s">
+      <c r="BQ5" s="833" t="s">
         <v>1837</v>
       </c>
       <c r="BR5" s="495" t="s">
@@ -32772,12 +32744,12 @@
     </row>
     <row r="6" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A6" s="165"/>
-      <c r="B6" s="873"/>
-      <c r="C6" s="806" t="s">
+      <c r="B6" s="872"/>
+      <c r="C6" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D6" s="208" t="s">
-        <v>2031</v>
+        <v>2051</v>
       </c>
       <c r="E6" s="224" t="s">
         <v>1756</v>
@@ -32899,8 +32871,8 @@
     </row>
     <row r="7" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A7" s="165"/>
-      <c r="B7" s="873"/>
-      <c r="C7" s="806" t="s">
+      <c r="B7" s="872"/>
+      <c r="C7" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D7" s="208" t="s">
@@ -33024,9 +32996,9 @@
       <c r="BV7" s="121"/>
       <c r="BW7" s="122"/>
     </row>
-    <row r="8" spans="1:75" s="773" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A8" s="777"/>
-      <c r="B8" s="873"/>
+    <row r="8" spans="1:75" s="772" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="776"/>
+      <c r="B8" s="872"/>
       <c r="C8" s="315" t="s">
         <v>1381</v>
       </c>
@@ -33163,8 +33135,8 @@
     </row>
     <row r="9" spans="1:75" s="203" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="202"/>
-      <c r="B9" s="873"/>
-      <c r="C9" s="817" t="s">
+      <c r="B9" s="872"/>
+      <c r="C9" s="816" t="s">
         <v>1311</v>
       </c>
       <c r="D9" s="729" t="s">
@@ -33201,7 +33173,7 @@
       <c r="Q9" s="119"/>
       <c r="R9" s="119"/>
       <c r="S9" s="128"/>
-      <c r="T9" s="843" t="s">
+      <c r="T9" s="842" t="s">
         <v>1978</v>
       </c>
       <c r="U9" s="718" t="s">
@@ -33266,7 +33238,7 @@
       <c r="AR9" s="421" t="s">
         <v>1979</v>
       </c>
-      <c r="AS9" s="842" t="s">
+      <c r="AS9" s="841" t="s">
         <v>1970</v>
       </c>
       <c r="AT9" s="132"/>
@@ -33311,7 +33283,7 @@
       <c r="BO9" s="119"/>
       <c r="BP9" s="119"/>
       <c r="BQ9" s="118"/>
-      <c r="BR9" s="841" t="s">
+      <c r="BR9" s="840" t="s">
         <v>1970</v>
       </c>
       <c r="BS9" s="183"/>
@@ -33322,8 +33294,8 @@
     </row>
     <row r="10" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A10" s="165"/>
-      <c r="B10" s="873"/>
-      <c r="C10" s="806" t="s">
+      <c r="B10" s="872"/>
+      <c r="C10" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D10" s="730" t="s">
@@ -33360,7 +33332,7 @@
       <c r="Q10" s="119"/>
       <c r="R10" s="119"/>
       <c r="S10" s="128"/>
-      <c r="T10" s="823" t="s">
+      <c r="T10" s="822" t="s">
         <v>1364</v>
       </c>
       <c r="U10" s="341" t="s">
@@ -33481,8 +33453,8 @@
     </row>
     <row r="11" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A11" s="165"/>
-      <c r="B11" s="873"/>
-      <c r="C11" s="806" t="s">
+      <c r="B11" s="872"/>
+      <c r="C11" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D11" s="730" t="s">
@@ -33519,7 +33491,7 @@
       <c r="Q11" s="119"/>
       <c r="R11" s="119"/>
       <c r="S11" s="128"/>
-      <c r="T11" s="823" t="s">
+      <c r="T11" s="822" t="s">
         <v>1944</v>
       </c>
       <c r="U11" s="341" t="s">
@@ -33638,13 +33610,13 @@
       <c r="BV11" s="364"/>
       <c r="BW11" s="146"/>
     </row>
-    <row r="12" spans="1:75" s="773" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A12" s="777"/>
-      <c r="B12" s="874"/>
+    <row r="12" spans="1:75" s="772" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A12" s="776"/>
+      <c r="B12" s="873"/>
       <c r="C12" s="164" t="s">
         <v>1381</v>
       </c>
-      <c r="D12" s="840" t="s">
+      <c r="D12" s="839" t="s">
         <v>1343</v>
       </c>
       <c r="E12" s="333" t="s">
@@ -33678,7 +33650,7 @@
       <c r="Q12" s="135"/>
       <c r="R12" s="135"/>
       <c r="S12" s="137"/>
-      <c r="T12" s="821" t="s">
+      <c r="T12" s="820" t="s">
         <v>1570</v>
       </c>
       <c r="U12" s="268" t="s">
@@ -33702,7 +33674,7 @@
       <c r="AA12" s="398" t="s">
         <v>1566</v>
       </c>
-      <c r="AB12" s="847" t="s">
+      <c r="AB12" s="846" t="s">
         <v>1569</v>
       </c>
       <c r="AC12" s="422" t="s">
@@ -33716,7 +33688,7 @@
       <c r="AG12" s="135"/>
       <c r="AH12" s="135"/>
       <c r="AI12" s="135"/>
-      <c r="AJ12" s="840" t="str">
+      <c r="AJ12" s="839" t="str">
         <f>D12</f>
         <v>대학C 101</v>
       </c>
@@ -33806,18 +33778,18 @@
       <c r="BR12" s="430" t="s">
         <v>1568</v>
       </c>
-      <c r="BS12" s="839"/>
-      <c r="BT12" s="839"/>
-      <c r="BU12" s="838"/>
-      <c r="BV12" s="838"/>
-      <c r="BW12" s="837"/>
+      <c r="BS12" s="838"/>
+      <c r="BT12" s="838"/>
+      <c r="BU12" s="837"/>
+      <c r="BV12" s="837"/>
+      <c r="BW12" s="836"/>
     </row>
     <row r="13" spans="1:75" s="203" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="202"/>
-      <c r="B13" s="872" t="s">
+      <c r="B13" s="871" t="s">
         <v>1932</v>
       </c>
-      <c r="C13" s="772" t="s">
+      <c r="C13" s="771" t="s">
         <v>1311</v>
       </c>
       <c r="D13" s="207" t="s">
@@ -33901,7 +33873,7 @@
       <c r="AF13" s="234" t="s">
         <v>1907</v>
       </c>
-      <c r="AG13" s="836" t="s">
+      <c r="AG13" s="835" t="s">
         <v>2023</v>
       </c>
       <c r="AH13" s="112"/>
@@ -33982,14 +33954,14 @@
       <c r="BK13" s="238" t="s">
         <v>1907</v>
       </c>
-      <c r="BL13" s="835" t="s">
+      <c r="BL13" s="834" t="s">
         <v>2023</v>
       </c>
       <c r="BM13" s="126"/>
       <c r="BN13" s="126"/>
       <c r="BO13" s="126"/>
       <c r="BP13" s="126"/>
-      <c r="BQ13" s="834" t="s">
+      <c r="BQ13" s="833" t="s">
         <v>1837</v>
       </c>
       <c r="BR13" s="495" t="s">
@@ -34009,8 +33981,8 @@
     </row>
     <row r="14" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A14" s="205"/>
-      <c r="B14" s="873"/>
-      <c r="C14" s="806" t="s">
+      <c r="B14" s="872"/>
+      <c r="C14" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D14" s="208" t="s">
@@ -34202,8 +34174,8 @@
     </row>
     <row r="15" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A15" s="205"/>
-      <c r="B15" s="873"/>
-      <c r="C15" s="806" t="s">
+      <c r="B15" s="872"/>
+      <c r="C15" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D15" s="208" t="s">
@@ -34393,9 +34365,9 @@
       <c r="BV15" s="132"/>
       <c r="BW15" s="122"/>
     </row>
-    <row r="16" spans="1:75" s="773" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A16" s="777"/>
-      <c r="B16" s="873"/>
+    <row r="16" spans="1:75" s="772" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A16" s="776"/>
+      <c r="B16" s="872"/>
       <c r="C16" s="315" t="s">
         <v>1381</v>
       </c>
@@ -34480,7 +34452,7 @@
       <c r="AF16" s="235" t="s">
         <v>1508</v>
       </c>
-      <c r="AG16" s="848" t="s">
+      <c r="AG16" s="847" t="s">
         <v>2027</v>
       </c>
       <c r="AH16" s="120"/>
@@ -34585,7 +34557,7 @@
         <f>AF16</f>
         <v>대학A 223</v>
       </c>
-      <c r="BL16" s="848" t="str">
+      <c r="BL16" s="847" t="str">
         <f>AG16</f>
         <v>대학A 228</v>
       </c>
@@ -34614,8 +34586,8 @@
     </row>
     <row r="17" spans="1:75" s="203" customFormat="1" ht="13.5" customHeight="1">
       <c r="A17" s="202"/>
-      <c r="B17" s="873"/>
-      <c r="C17" s="817" t="s">
+      <c r="B17" s="872"/>
+      <c r="C17" s="816" t="s">
         <v>1311</v>
       </c>
       <c r="D17" s="257" t="s">
@@ -34627,7 +34599,7 @@
       <c r="F17" s="263" t="s">
         <v>200</v>
       </c>
-      <c r="G17" s="833" t="s">
+      <c r="G17" s="832" t="s">
         <v>1859</v>
       </c>
       <c r="H17" s="343" t="s">
@@ -34664,7 +34636,7 @@
         <v>1849</v>
       </c>
       <c r="S17" s="124"/>
-      <c r="T17" s="831" t="s">
+      <c r="T17" s="830" t="s">
         <v>181</v>
       </c>
       <c r="U17" s="259" t="s">
@@ -34797,7 +34769,7 @@
       <c r="BN17" s="123"/>
       <c r="BO17" s="123"/>
       <c r="BP17" s="123"/>
-      <c r="BQ17" s="832" t="s">
+      <c r="BQ17" s="831" t="s">
         <v>1837</v>
       </c>
       <c r="BR17" s="129"/>
@@ -34809,8 +34781,8 @@
     </row>
     <row r="18" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A18" s="205"/>
-      <c r="B18" s="873"/>
-      <c r="C18" s="806" t="s">
+      <c r="B18" s="872"/>
+      <c r="C18" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D18" s="257" t="s">
@@ -34859,7 +34831,7 @@
         <v>1824</v>
       </c>
       <c r="S18" s="167"/>
-      <c r="T18" s="831" t="s">
+      <c r="T18" s="830" t="s">
         <v>1364</v>
       </c>
       <c r="U18" s="259" t="s">
@@ -35006,8 +34978,8 @@
     </row>
     <row r="19" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A19" s="205"/>
-      <c r="B19" s="873"/>
-      <c r="C19" s="806" t="s">
+      <c r="B19" s="872"/>
+      <c r="C19" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D19" s="257" t="s">
@@ -35056,7 +35028,7 @@
         <v>1794</v>
       </c>
       <c r="S19" s="167"/>
-      <c r="T19" s="831" t="s">
+      <c r="T19" s="830" t="s">
         <v>1793</v>
       </c>
       <c r="U19" s="259" t="s">
@@ -35199,16 +35171,16 @@
       <c r="BV19" s="366"/>
       <c r="BW19" s="130"/>
     </row>
-    <row r="20" spans="1:75" s="773" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="777"/>
-      <c r="B20" s="874"/>
+    <row r="20" spans="1:75" s="772" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A20" s="776"/>
+      <c r="B20" s="873"/>
       <c r="C20" s="138" t="s">
         <v>1381</v>
       </c>
       <c r="D20" s="258" t="s">
         <v>1343</v>
       </c>
-      <c r="E20" s="857" t="s">
+      <c r="E20" s="856" t="s">
         <v>2050</v>
       </c>
       <c r="F20" s="264" t="s">
@@ -35251,7 +35223,7 @@
         <v>1776</v>
       </c>
       <c r="S20" s="138"/>
-      <c r="T20" s="830" t="s">
+      <c r="T20" s="829" t="s">
         <v>1345</v>
       </c>
       <c r="U20" s="261" t="s">
@@ -35297,12 +35269,12 @@
         <f>AD12</f>
         <v>다산 615</v>
       </c>
-      <c r="AI20" s="829"/>
+      <c r="AI20" s="828"/>
       <c r="AJ20" s="258" t="str">
         <f>D20</f>
         <v>대학C 101</v>
       </c>
-      <c r="AK20" s="857" t="str">
+      <c r="AK20" s="856" t="str">
         <f>E20</f>
         <v>대학A 229</v>
       </c>
@@ -35413,96 +35385,96 @@
       <c r="BQ20" s="139" t="s">
         <v>1334</v>
       </c>
-      <c r="BR20" s="766"/>
-      <c r="BS20" s="766"/>
-      <c r="BT20" s="766"/>
-      <c r="BU20" s="767"/>
-      <c r="BV20" s="767"/>
-      <c r="BW20" s="820"/>
+      <c r="BR20" s="765"/>
+      <c r="BS20" s="765"/>
+      <c r="BT20" s="765"/>
+      <c r="BU20" s="766"/>
+      <c r="BV20" s="766"/>
+      <c r="BW20" s="819"/>
     </row>
     <row r="21" spans="1:75" s="203" customFormat="1" ht="18" thickBot="1">
       <c r="A21" s="165"/>
-      <c r="B21" s="897"/>
-      <c r="C21" s="898"/>
-      <c r="D21" s="898"/>
-      <c r="E21" s="898"/>
-      <c r="F21" s="898"/>
-      <c r="G21" s="898"/>
-      <c r="H21" s="898"/>
-      <c r="I21" s="898"/>
-      <c r="J21" s="898"/>
-      <c r="K21" s="898"/>
-      <c r="L21" s="898"/>
-      <c r="M21" s="898"/>
-      <c r="N21" s="898"/>
-      <c r="O21" s="898"/>
-      <c r="P21" s="898"/>
-      <c r="Q21" s="898"/>
-      <c r="R21" s="898"/>
-      <c r="S21" s="898"/>
-      <c r="T21" s="898"/>
-      <c r="U21" s="898"/>
-      <c r="V21" s="898"/>
-      <c r="W21" s="898"/>
-      <c r="X21" s="898"/>
-      <c r="Y21" s="898"/>
-      <c r="Z21" s="898"/>
-      <c r="AA21" s="898"/>
-      <c r="AB21" s="898"/>
-      <c r="AC21" s="898"/>
-      <c r="AD21" s="898"/>
-      <c r="AE21" s="898"/>
-      <c r="AF21" s="898"/>
-      <c r="AG21" s="898"/>
-      <c r="AH21" s="898"/>
-      <c r="AI21" s="898"/>
-      <c r="AJ21" s="898"/>
-      <c r="AK21" s="898"/>
-      <c r="AL21" s="898"/>
-      <c r="AM21" s="898"/>
-      <c r="AN21" s="898"/>
-      <c r="AO21" s="898"/>
-      <c r="AP21" s="898"/>
-      <c r="AQ21" s="898"/>
-      <c r="AR21" s="898"/>
-      <c r="AS21" s="898"/>
-      <c r="AT21" s="898"/>
-      <c r="AU21" s="898"/>
-      <c r="AV21" s="898"/>
-      <c r="AW21" s="898"/>
-      <c r="AX21" s="898"/>
-      <c r="AY21" s="898"/>
-      <c r="AZ21" s="898"/>
-      <c r="BA21" s="898"/>
-      <c r="BB21" s="898"/>
-      <c r="BC21" s="898"/>
-      <c r="BD21" s="898"/>
-      <c r="BE21" s="898"/>
-      <c r="BF21" s="898"/>
-      <c r="BG21" s="898"/>
-      <c r="BH21" s="898"/>
-      <c r="BI21" s="898"/>
-      <c r="BJ21" s="898"/>
-      <c r="BK21" s="898"/>
-      <c r="BL21" s="898"/>
-      <c r="BM21" s="898"/>
-      <c r="BN21" s="898"/>
-      <c r="BO21" s="898"/>
-      <c r="BP21" s="898"/>
-      <c r="BQ21" s="898"/>
-      <c r="BR21" s="898"/>
-      <c r="BS21" s="898"/>
-      <c r="BT21" s="898"/>
-      <c r="BU21" s="898"/>
-      <c r="BV21" s="898"/>
-      <c r="BW21" s="898"/>
+      <c r="B21" s="896"/>
+      <c r="C21" s="897"/>
+      <c r="D21" s="897"/>
+      <c r="E21" s="897"/>
+      <c r="F21" s="897"/>
+      <c r="G21" s="897"/>
+      <c r="H21" s="897"/>
+      <c r="I21" s="897"/>
+      <c r="J21" s="897"/>
+      <c r="K21" s="897"/>
+      <c r="L21" s="897"/>
+      <c r="M21" s="897"/>
+      <c r="N21" s="897"/>
+      <c r="O21" s="897"/>
+      <c r="P21" s="897"/>
+      <c r="Q21" s="897"/>
+      <c r="R21" s="897"/>
+      <c r="S21" s="897"/>
+      <c r="T21" s="897"/>
+      <c r="U21" s="897"/>
+      <c r="V21" s="897"/>
+      <c r="W21" s="897"/>
+      <c r="X21" s="897"/>
+      <c r="Y21" s="897"/>
+      <c r="Z21" s="897"/>
+      <c r="AA21" s="897"/>
+      <c r="AB21" s="897"/>
+      <c r="AC21" s="897"/>
+      <c r="AD21" s="897"/>
+      <c r="AE21" s="897"/>
+      <c r="AF21" s="897"/>
+      <c r="AG21" s="897"/>
+      <c r="AH21" s="897"/>
+      <c r="AI21" s="897"/>
+      <c r="AJ21" s="897"/>
+      <c r="AK21" s="897"/>
+      <c r="AL21" s="897"/>
+      <c r="AM21" s="897"/>
+      <c r="AN21" s="897"/>
+      <c r="AO21" s="897"/>
+      <c r="AP21" s="897"/>
+      <c r="AQ21" s="897"/>
+      <c r="AR21" s="897"/>
+      <c r="AS21" s="897"/>
+      <c r="AT21" s="897"/>
+      <c r="AU21" s="897"/>
+      <c r="AV21" s="897"/>
+      <c r="AW21" s="897"/>
+      <c r="AX21" s="897"/>
+      <c r="AY21" s="897"/>
+      <c r="AZ21" s="897"/>
+      <c r="BA21" s="897"/>
+      <c r="BB21" s="897"/>
+      <c r="BC21" s="897"/>
+      <c r="BD21" s="897"/>
+      <c r="BE21" s="897"/>
+      <c r="BF21" s="897"/>
+      <c r="BG21" s="897"/>
+      <c r="BH21" s="897"/>
+      <c r="BI21" s="897"/>
+      <c r="BJ21" s="897"/>
+      <c r="BK21" s="897"/>
+      <c r="BL21" s="897"/>
+      <c r="BM21" s="897"/>
+      <c r="BN21" s="897"/>
+      <c r="BO21" s="897"/>
+      <c r="BP21" s="897"/>
+      <c r="BQ21" s="897"/>
+      <c r="BR21" s="897"/>
+      <c r="BS21" s="897"/>
+      <c r="BT21" s="897"/>
+      <c r="BU21" s="897"/>
+      <c r="BV21" s="897"/>
+      <c r="BW21" s="897"/>
     </row>
     <row r="22" spans="1:75" s="203" customFormat="1" ht="13.5" customHeight="1">
       <c r="A22" s="202"/>
-      <c r="B22" s="872" t="s">
+      <c r="B22" s="871" t="s">
         <v>1770</v>
       </c>
-      <c r="C22" s="772" t="s">
+      <c r="C22" s="771" t="s">
         <v>1311</v>
       </c>
       <c r="D22" s="207" t="s">
@@ -35562,7 +35534,7 @@
       <c r="AJ22" s="207" t="s">
         <v>1768</v>
       </c>
-      <c r="AK22" s="812" t="s">
+      <c r="AK22" s="811" t="s">
         <v>1767</v>
       </c>
       <c r="AL22" s="307" t="s">
@@ -35612,7 +35584,7 @@
       <c r="BN22" s="114"/>
       <c r="BO22" s="114"/>
       <c r="BP22" s="114"/>
-      <c r="BQ22" s="828"/>
+      <c r="BQ22" s="827"/>
       <c r="BR22" s="515" t="s">
         <v>1670</v>
       </c>
@@ -35628,8 +35600,8 @@
     </row>
     <row r="23" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A23" s="205"/>
-      <c r="B23" s="873"/>
-      <c r="C23" s="806" t="s">
+      <c r="B23" s="872"/>
+      <c r="C23" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D23" s="208" t="s">
@@ -35755,8 +35727,8 @@
     </row>
     <row r="24" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A24" s="205"/>
-      <c r="B24" s="873"/>
-      <c r="C24" s="806" t="s">
+      <c r="B24" s="872"/>
+      <c r="C24" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D24" s="208" t="s">
@@ -35880,9 +35852,9 @@
       <c r="BV24" s="121"/>
       <c r="BW24" s="122"/>
     </row>
-    <row r="25" spans="1:75" s="825" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A25" s="805"/>
-      <c r="B25" s="873"/>
+    <row r="25" spans="1:75" s="824" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A25" s="804"/>
+      <c r="B25" s="872"/>
       <c r="C25" s="315" t="s">
         <v>1381</v>
       </c>
@@ -35895,7 +35867,7 @@
       <c r="F25" s="224" t="s">
         <v>1341</v>
       </c>
-      <c r="G25" s="826" t="s">
+      <c r="G25" s="825" t="s">
         <v>1507</v>
       </c>
       <c r="H25" s="235" t="s">
@@ -35906,7 +35878,7 @@
       </c>
       <c r="J25" s="160"/>
       <c r="K25" s="160"/>
-      <c r="L25" s="827"/>
+      <c r="L25" s="826"/>
       <c r="M25" s="119"/>
       <c r="N25" s="120"/>
       <c r="O25" s="120"/>
@@ -35948,11 +35920,11 @@
         <f>E25</f>
         <v>대학A 229</v>
       </c>
-      <c r="AL25" s="826" t="str">
+      <c r="AL25" s="825" t="str">
         <f>F25</f>
         <v>대학A 224</v>
       </c>
-      <c r="AM25" s="826" t="s">
+      <c r="AM25" s="825" t="s">
         <v>1507</v>
       </c>
       <c r="AN25" s="235" t="s">
@@ -36017,8 +35989,8 @@
     </row>
     <row r="26" spans="1:75" s="203" customFormat="1" ht="13.5" customHeight="1">
       <c r="A26" s="202"/>
-      <c r="B26" s="873"/>
-      <c r="C26" s="817" t="s">
+      <c r="B26" s="872"/>
+      <c r="C26" s="816" t="s">
         <v>1311</v>
       </c>
       <c r="D26" s="257" t="s">
@@ -36048,7 +36020,7 @@
       <c r="L26" s="702" t="s">
         <v>1731</v>
       </c>
-      <c r="M26" s="824" t="s">
+      <c r="M26" s="823" t="s">
         <v>1730</v>
       </c>
       <c r="N26" s="388" t="s">
@@ -36061,7 +36033,7 @@
       <c r="Q26" s="132"/>
       <c r="R26" s="132"/>
       <c r="S26" s="128"/>
-      <c r="T26" s="823" t="s">
+      <c r="T26" s="822" t="s">
         <v>1727</v>
       </c>
       <c r="U26" s="263" t="s">
@@ -36127,7 +36099,7 @@
       <c r="AS26" s="702" t="s">
         <v>1731</v>
       </c>
-      <c r="AT26" s="824" t="s">
+      <c r="AT26" s="823" t="s">
         <v>1730</v>
       </c>
       <c r="AU26" s="388" t="s">
@@ -36141,7 +36113,7 @@
       </c>
       <c r="AX26" s="132"/>
       <c r="AY26" s="128"/>
-      <c r="AZ26" s="823" t="s">
+      <c r="AZ26" s="822" t="s">
         <v>1727</v>
       </c>
       <c r="BA26" s="354" t="s">
@@ -36192,8 +36164,8 @@
     </row>
     <row r="27" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A27" s="205"/>
-      <c r="B27" s="873"/>
-      <c r="C27" s="806" t="s">
+      <c r="B27" s="872"/>
+      <c r="C27" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D27" s="257" t="s">
@@ -36236,7 +36208,7 @@
       <c r="Q27" s="132"/>
       <c r="R27" s="132"/>
       <c r="S27" s="128"/>
-      <c r="T27" s="823" t="s">
+      <c r="T27" s="822" t="s">
         <v>1715</v>
       </c>
       <c r="U27" s="263" t="s">
@@ -36316,7 +36288,7 @@
       </c>
       <c r="AX27" s="132"/>
       <c r="AY27" s="128"/>
-      <c r="AZ27" s="823" t="s">
+      <c r="AZ27" s="822" t="s">
         <v>1715</v>
       </c>
       <c r="BA27" s="354" t="s">
@@ -36367,8 +36339,8 @@
     </row>
     <row r="28" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A28" s="205"/>
-      <c r="B28" s="873"/>
-      <c r="C28" s="806" t="s">
+      <c r="B28" s="872"/>
+      <c r="C28" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D28" s="257" t="s">
@@ -36411,7 +36383,7 @@
       <c r="Q28" s="132"/>
       <c r="R28" s="132"/>
       <c r="S28" s="128"/>
-      <c r="T28" s="823" t="s">
+      <c r="T28" s="822" t="s">
         <v>1697</v>
       </c>
       <c r="U28" s="263" t="s">
@@ -36491,7 +36463,7 @@
       </c>
       <c r="AX28" s="132"/>
       <c r="AY28" s="128"/>
-      <c r="AZ28" s="823" t="s">
+      <c r="AZ28" s="822" t="s">
         <v>1697</v>
       </c>
       <c r="BA28" s="354" t="s">
@@ -36540,9 +36512,9 @@
       </c>
       <c r="BW28" s="130"/>
     </row>
-    <row r="29" spans="1:75" s="773" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A29" s="777"/>
-      <c r="B29" s="874"/>
+    <row r="29" spans="1:75" s="772" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A29" s="776"/>
+      <c r="B29" s="873"/>
       <c r="C29" s="164" t="s">
         <v>1381</v>
       </c>
@@ -36576,17 +36548,17 @@
       <c r="M29" s="378" t="s">
         <v>1690</v>
       </c>
-      <c r="N29" s="845" t="s">
+      <c r="N29" s="844" t="s">
         <v>2025</v>
       </c>
-      <c r="O29" s="844" t="s">
+      <c r="O29" s="843" t="s">
         <v>2024</v>
       </c>
       <c r="P29" s="136"/>
       <c r="Q29" s="136"/>
       <c r="R29" s="136"/>
       <c r="S29" s="137"/>
-      <c r="T29" s="850" t="s">
+      <c r="T29" s="849" t="s">
         <v>2030</v>
       </c>
       <c r="U29" s="267" t="s">
@@ -36627,7 +36599,7 @@
         <f t="shared" ref="AJ29:AO29" si="6">D29</f>
         <v>대학C 112</v>
       </c>
-      <c r="AK29" s="822" t="str">
+      <c r="AK29" s="821" t="str">
         <f t="shared" si="6"/>
         <v>대학C 101</v>
       </c>
@@ -36666,11 +36638,11 @@
         <f t="shared" si="7"/>
         <v>기계 101</v>
       </c>
-      <c r="AU29" s="845" t="str">
+      <c r="AU29" s="844" t="str">
         <f t="shared" si="7"/>
         <v>대학A 101</v>
       </c>
-      <c r="AV29" s="844" t="str">
+      <c r="AV29" s="843" t="str">
         <f t="shared" si="7"/>
         <v>대학A 114</v>
       </c>
@@ -36679,7 +36651,7 @@
       </c>
       <c r="AX29" s="136"/>
       <c r="AY29" s="137"/>
-      <c r="AZ29" s="851" t="str">
+      <c r="AZ29" s="850" t="str">
         <f>T29</f>
         <v>대학C 501</v>
       </c>
@@ -36720,8 +36692,8 @@
       <c r="BQ29" s="359" t="s">
         <v>1687</v>
       </c>
-      <c r="BR29" s="766"/>
-      <c r="BS29" s="766"/>
+      <c r="BR29" s="765"/>
+      <c r="BS29" s="765"/>
       <c r="BT29" s="344" t="s">
         <v>1636</v>
       </c>
@@ -36731,20 +36703,20 @@
       <c r="BV29" s="279" t="s">
         <v>1567</v>
       </c>
-      <c r="BW29" s="820"/>
+      <c r="BW29" s="819"/>
     </row>
     <row r="30" spans="1:75" s="203" customFormat="1" ht="17.25" customHeight="1">
       <c r="A30" s="202"/>
-      <c r="B30" s="872" t="s">
+      <c r="B30" s="871" t="s">
         <v>1686</v>
       </c>
-      <c r="C30" s="772" t="s">
+      <c r="C30" s="771" t="s">
         <v>1311</v>
       </c>
       <c r="D30" s="207" t="s">
         <v>1685</v>
       </c>
-      <c r="E30" s="812" t="s">
+      <c r="E30" s="811" t="s">
         <v>1563</v>
       </c>
       <c r="F30" s="217" t="s">
@@ -36810,7 +36782,7 @@
       <c r="AJ30" s="207" t="s">
         <v>1685</v>
       </c>
-      <c r="AK30" s="812" t="s">
+      <c r="AK30" s="811" t="s">
         <v>1563</v>
       </c>
       <c r="AL30" s="217" t="s">
@@ -36890,8 +36862,8 @@
     </row>
     <row r="31" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A31" s="205"/>
-      <c r="B31" s="873"/>
-      <c r="C31" s="806" t="s">
+      <c r="B31" s="872"/>
+      <c r="C31" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D31" s="208" t="s">
@@ -37043,8 +37015,8 @@
     </row>
     <row r="32" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A32" s="205"/>
-      <c r="B32" s="873"/>
-      <c r="C32" s="806" t="s">
+      <c r="B32" s="872"/>
+      <c r="C32" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D32" s="208" t="s">
@@ -37194,9 +37166,9 @@
       <c r="BV32" s="132"/>
       <c r="BW32" s="146"/>
     </row>
-    <row r="33" spans="1:75" s="773" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="777"/>
-      <c r="B33" s="873"/>
+    <row r="33" spans="1:75" s="772" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="776"/>
+      <c r="B33" s="872"/>
       <c r="C33" s="315" t="s">
         <v>1381</v>
       </c>
@@ -37229,11 +37201,11 @@
       </c>
       <c r="M33" s="120"/>
       <c r="N33" s="120"/>
-      <c r="O33" s="819"/>
-      <c r="P33" s="819"/>
-      <c r="Q33" s="818"/>
-      <c r="R33" s="818"/>
-      <c r="S33" s="818"/>
+      <c r="O33" s="818"/>
+      <c r="P33" s="818"/>
+      <c r="Q33" s="817"/>
+      <c r="R33" s="817"/>
+      <c r="S33" s="817"/>
       <c r="T33" s="208" t="s">
         <v>1425</v>
       </c>
@@ -37366,8 +37338,8 @@
     </row>
     <row r="34" spans="1:75" s="203" customFormat="1" ht="13.5" customHeight="1">
       <c r="A34" s="202"/>
-      <c r="B34" s="873"/>
-      <c r="C34" s="817" t="s">
+      <c r="B34" s="872"/>
+      <c r="C34" s="816" t="s">
         <v>1311</v>
       </c>
       <c r="D34" s="335" t="s">
@@ -37553,8 +37525,8 @@
     </row>
     <row r="35" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A35" s="205"/>
-      <c r="B35" s="873"/>
-      <c r="C35" s="806" t="s">
+      <c r="B35" s="872"/>
+      <c r="C35" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D35" s="335" t="s">
@@ -37740,8 +37712,8 @@
     </row>
     <row r="36" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A36" s="205"/>
-      <c r="B36" s="873"/>
-      <c r="C36" s="806" t="s">
+      <c r="B36" s="872"/>
+      <c r="C36" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D36" s="335" t="s">
@@ -37925,9 +37897,9 @@
       </c>
       <c r="BW36" s="128"/>
     </row>
-    <row r="37" spans="1:75" s="773" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A37" s="777"/>
-      <c r="B37" s="874"/>
+    <row r="37" spans="1:75" s="772" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A37" s="776"/>
+      <c r="B37" s="873"/>
       <c r="C37" s="138" t="s">
         <v>1381</v>
       </c>
@@ -37973,8 +37945,8 @@
       <c r="Q37" s="479" t="s">
         <v>1568</v>
       </c>
-      <c r="R37" s="816"/>
-      <c r="S37" s="816"/>
+      <c r="R37" s="815"/>
+      <c r="S37" s="815"/>
       <c r="T37" s="258" t="s">
         <v>1345</v>
       </c>
@@ -38053,7 +38025,7 @@
         <f t="shared" si="10"/>
         <v>대학A 114</v>
       </c>
-      <c r="AU37" s="815" t="str">
+      <c r="AU37" s="814" t="str">
         <f t="shared" si="10"/>
         <v>대학A 102</v>
       </c>
@@ -38061,7 +38033,7 @@
         <f t="shared" si="10"/>
         <v>지환 410</v>
       </c>
-      <c r="AW37" s="814" t="s">
+      <c r="AW37" s="813" t="s">
         <v>1429</v>
       </c>
       <c r="AX37" s="424" t="s">
@@ -38137,16 +38109,16 @@
     </row>
     <row r="38" spans="1:75" s="203" customFormat="1" ht="15.75" customHeight="1">
       <c r="A38" s="202"/>
-      <c r="B38" s="872" t="s">
+      <c r="B38" s="871" t="s">
         <v>501</v>
       </c>
-      <c r="C38" s="813" t="s">
+      <c r="C38" s="812" t="s">
         <v>1311</v>
       </c>
       <c r="D38" s="219" t="s">
         <v>1564</v>
       </c>
-      <c r="E38" s="812" t="s">
+      <c r="E38" s="811" t="s">
         <v>1562</v>
       </c>
       <c r="F38" s="209" t="s">
@@ -38204,7 +38176,7 @@
       <c r="AJ38" s="219" t="s">
         <v>1564</v>
       </c>
-      <c r="AK38" s="812" t="s">
+      <c r="AK38" s="811" t="s">
         <v>1563</v>
       </c>
       <c r="AL38" s="209" t="s">
@@ -38237,7 +38209,7 @@
       <c r="AW38" s="112"/>
       <c r="AX38" s="112"/>
       <c r="AY38" s="156"/>
-      <c r="AZ38" s="811"/>
+      <c r="AZ38" s="810"/>
       <c r="BA38" s="114"/>
       <c r="BB38" s="114"/>
       <c r="BC38" s="112"/>
@@ -38252,28 +38224,28 @@
         <v>1479</v>
       </c>
       <c r="BH38" s="112"/>
-      <c r="BI38" s="810" t="s">
+      <c r="BI38" s="809" t="s">
         <v>1553</v>
       </c>
-      <c r="BJ38" s="810" t="s">
+      <c r="BJ38" s="809" t="s">
         <v>1552</v>
       </c>
-      <c r="BK38" s="810" t="s">
+      <c r="BK38" s="809" t="s">
         <v>1551</v>
       </c>
-      <c r="BL38" s="810" t="s">
+      <c r="BL38" s="809" t="s">
         <v>1550</v>
       </c>
-      <c r="BM38" s="810" t="s">
+      <c r="BM38" s="809" t="s">
         <v>1549</v>
       </c>
-      <c r="BN38" s="810" t="s">
+      <c r="BN38" s="809" t="s">
         <v>1548</v>
       </c>
-      <c r="BO38" s="810" t="s">
+      <c r="BO38" s="809" t="s">
         <v>1547</v>
       </c>
-      <c r="BP38" s="809" t="s">
+      <c r="BP38" s="808" t="s">
         <v>1546</v>
       </c>
       <c r="BQ38" s="700"/>
@@ -38288,8 +38260,8 @@
     </row>
     <row r="39" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A39" s="205"/>
-      <c r="B39" s="873"/>
-      <c r="C39" s="806" t="s">
+      <c r="B39" s="872"/>
+      <c r="C39" s="805" t="s">
         <v>1478</v>
       </c>
       <c r="D39" s="208" t="s">
@@ -38401,28 +38373,28 @@
         <v>1535</v>
       </c>
       <c r="BH39" s="120"/>
-      <c r="BI39" s="808" t="s">
+      <c r="BI39" s="807" t="s">
         <v>1534</v>
       </c>
-      <c r="BJ39" s="793" t="s">
+      <c r="BJ39" s="792" t="s">
         <v>1533</v>
       </c>
-      <c r="BK39" s="793" t="s">
+      <c r="BK39" s="792" t="s">
         <v>1532</v>
       </c>
-      <c r="BL39" s="793" t="s">
+      <c r="BL39" s="792" t="s">
         <v>1531</v>
       </c>
-      <c r="BM39" s="793" t="s">
+      <c r="BM39" s="792" t="s">
         <v>1530</v>
       </c>
-      <c r="BN39" s="793" t="s">
+      <c r="BN39" s="792" t="s">
         <v>1529</v>
       </c>
-      <c r="BO39" s="793" t="s">
+      <c r="BO39" s="792" t="s">
         <v>1528</v>
       </c>
-      <c r="BP39" s="807" t="s">
+      <c r="BP39" s="806" t="s">
         <v>1527</v>
       </c>
       <c r="BQ39" s="701"/>
@@ -38437,8 +38409,8 @@
     </row>
     <row r="40" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A40" s="205"/>
-      <c r="B40" s="873"/>
-      <c r="C40" s="806" t="s">
+      <c r="B40" s="872"/>
+      <c r="C40" s="805" t="s">
         <v>1454</v>
       </c>
       <c r="D40" s="220" t="s">
@@ -38550,28 +38522,28 @@
         <v>2026</v>
       </c>
       <c r="BH40" s="120"/>
-      <c r="BI40" s="788" t="s">
+      <c r="BI40" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BJ40" s="788" t="s">
+      <c r="BJ40" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BK40" s="788" t="s">
+      <c r="BK40" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BL40" s="788" t="s">
+      <c r="BL40" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BM40" s="788" t="s">
+      <c r="BM40" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BN40" s="788" t="s">
+      <c r="BN40" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BO40" s="788" t="s">
+      <c r="BO40" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BP40" s="787" t="s">
+      <c r="BP40" s="786" t="s">
         <v>1439</v>
       </c>
       <c r="BQ40" s="701"/>
@@ -38584,9 +38556,9 @@
       <c r="BV40" s="119"/>
       <c r="BW40" s="146"/>
     </row>
-    <row r="41" spans="1:75" s="799" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="805"/>
-      <c r="B41" s="873"/>
+    <row r="41" spans="1:75" s="798" customFormat="1" ht="15" customHeight="1">
+      <c r="A41" s="804"/>
+      <c r="B41" s="872"/>
       <c r="C41" s="315" t="s">
         <v>1381</v>
       </c>
@@ -38690,7 +38662,7 @@
         <f>N41</f>
         <v>대학A 223</v>
       </c>
-      <c r="AT41" s="804"/>
+      <c r="AT41" s="803"/>
       <c r="AU41" s="120"/>
       <c r="AV41" s="120"/>
       <c r="AW41" s="120"/>
@@ -38707,36 +38679,36 @@
       <c r="BF41" s="272" t="s">
         <v>1263</v>
       </c>
-      <c r="BG41" s="846" t="str">
+      <c r="BG41" s="845" t="str">
         <f>BV45</f>
         <v>대학B 115</v>
       </c>
       <c r="BH41" s="120"/>
-      <c r="BI41" s="803" t="s">
+      <c r="BI41" s="802" t="s">
         <v>1434</v>
       </c>
-      <c r="BJ41" s="803" t="s">
+      <c r="BJ41" s="802" t="s">
         <v>1435</v>
       </c>
-      <c r="BK41" s="802" t="s">
+      <c r="BK41" s="801" t="s">
         <v>1380</v>
       </c>
-      <c r="BL41" s="802" t="s">
+      <c r="BL41" s="801" t="s">
         <v>1379</v>
       </c>
-      <c r="BM41" s="802" t="s">
+      <c r="BM41" s="801" t="s">
         <v>1507</v>
       </c>
-      <c r="BN41" s="802" t="s">
+      <c r="BN41" s="801" t="s">
         <v>1506</v>
       </c>
-      <c r="BO41" s="802" t="s">
+      <c r="BO41" s="801" t="s">
         <v>1337</v>
       </c>
-      <c r="BP41" s="801" t="s">
+      <c r="BP41" s="800" t="s">
         <v>1504</v>
       </c>
-      <c r="BQ41" s="800"/>
+      <c r="BQ41" s="799"/>
       <c r="BR41" s="517" t="s">
         <v>814</v>
       </c>
@@ -38746,9 +38718,9 @@
       <c r="BV41" s="119"/>
       <c r="BW41" s="169"/>
     </row>
-    <row r="42" spans="1:75" s="773" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A42" s="798"/>
-      <c r="B42" s="873"/>
+    <row r="42" spans="1:75" s="772" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A42" s="797"/>
+      <c r="B42" s="872"/>
       <c r="C42" s="170" t="s">
         <v>1311</v>
       </c>
@@ -38767,7 +38739,7 @@
       <c r="H42" s="345" t="s">
         <v>1495</v>
       </c>
-      <c r="I42" s="797" t="s">
+      <c r="I42" s="796" t="s">
         <v>1494</v>
       </c>
       <c r="J42" s="375" t="s">
@@ -38823,7 +38795,7 @@
       <c r="AN42" s="345" t="s">
         <v>1495</v>
       </c>
-      <c r="AO42" s="797" t="s">
+      <c r="AO42" s="796" t="s">
         <v>1494</v>
       </c>
       <c r="AP42" s="274" t="s">
@@ -38844,39 +38816,39 @@
       <c r="AW42" s="119"/>
       <c r="AX42" s="119"/>
       <c r="AY42" s="132"/>
-      <c r="AZ42" s="904" t="s">
+      <c r="AZ42" s="900" t="s">
         <v>1491</v>
       </c>
-      <c r="BA42" s="905"/>
-      <c r="BB42" s="905"/>
-      <c r="BC42" s="905"/>
-      <c r="BD42" s="905"/>
-      <c r="BE42" s="905"/>
-      <c r="BF42" s="905"/>
-      <c r="BG42" s="905"/>
-      <c r="BH42" s="906"/>
-      <c r="BI42" s="796" t="s">
+      <c r="BA42" s="901"/>
+      <c r="BB42" s="901"/>
+      <c r="BC42" s="901"/>
+      <c r="BD42" s="901"/>
+      <c r="BE42" s="901"/>
+      <c r="BF42" s="901"/>
+      <c r="BG42" s="901"/>
+      <c r="BH42" s="902"/>
+      <c r="BI42" s="795" t="s">
         <v>1490</v>
       </c>
-      <c r="BJ42" s="796" t="s">
+      <c r="BJ42" s="795" t="s">
         <v>1489</v>
       </c>
-      <c r="BK42" s="795" t="s">
+      <c r="BK42" s="794" t="s">
         <v>1488</v>
       </c>
-      <c r="BL42" s="795" t="s">
+      <c r="BL42" s="794" t="s">
         <v>1487</v>
       </c>
-      <c r="BM42" s="795" t="s">
+      <c r="BM42" s="794" t="s">
         <v>1486</v>
       </c>
-      <c r="BN42" s="795" t="s">
+      <c r="BN42" s="794" t="s">
         <v>1485</v>
       </c>
-      <c r="BO42" s="795" t="s">
+      <c r="BO42" s="794" t="s">
         <v>1484</v>
       </c>
-      <c r="BP42" s="794" t="s">
+      <c r="BP42" s="793" t="s">
         <v>1483</v>
       </c>
       <c r="BQ42" s="358" t="s">
@@ -38897,10 +38869,10 @@
       </c>
       <c r="BW42" s="167"/>
     </row>
-    <row r="43" spans="1:75" s="773" customFormat="1" ht="23.1" customHeight="1">
+    <row r="43" spans="1:75" s="772" customFormat="1" ht="23.1" customHeight="1">
       <c r="A43" s="205"/>
-      <c r="B43" s="873"/>
-      <c r="C43" s="789" t="s">
+      <c r="B43" s="872"/>
+      <c r="C43" s="788" t="s">
         <v>1478</v>
       </c>
       <c r="D43" s="263" t="s">
@@ -38995,39 +38967,39 @@
       <c r="AW43" s="119"/>
       <c r="AX43" s="119"/>
       <c r="AY43" s="132"/>
-      <c r="AZ43" s="875" t="s">
+      <c r="AZ43" s="874" t="s">
         <v>1466</v>
       </c>
-      <c r="BA43" s="876"/>
-      <c r="BB43" s="876"/>
-      <c r="BC43" s="876"/>
-      <c r="BD43" s="876"/>
-      <c r="BE43" s="876"/>
-      <c r="BF43" s="876"/>
-      <c r="BG43" s="876"/>
-      <c r="BH43" s="877"/>
-      <c r="BI43" s="793" t="s">
+      <c r="BA43" s="875"/>
+      <c r="BB43" s="875"/>
+      <c r="BC43" s="875"/>
+      <c r="BD43" s="875"/>
+      <c r="BE43" s="875"/>
+      <c r="BF43" s="875"/>
+      <c r="BG43" s="875"/>
+      <c r="BH43" s="876"/>
+      <c r="BI43" s="792" t="s">
         <v>1465</v>
       </c>
-      <c r="BJ43" s="793" t="s">
+      <c r="BJ43" s="792" t="s">
         <v>1464</v>
       </c>
-      <c r="BK43" s="792" t="s">
+      <c r="BK43" s="791" t="s">
         <v>1463</v>
       </c>
-      <c r="BL43" s="792" t="s">
+      <c r="BL43" s="791" t="s">
         <v>1462</v>
       </c>
-      <c r="BM43" s="792" t="s">
+      <c r="BM43" s="791" t="s">
         <v>1461</v>
       </c>
-      <c r="BN43" s="792" t="s">
+      <c r="BN43" s="791" t="s">
         <v>1460</v>
       </c>
-      <c r="BO43" s="792" t="s">
+      <c r="BO43" s="791" t="s">
         <v>1459</v>
       </c>
-      <c r="BP43" s="791" t="s">
+      <c r="BP43" s="790" t="s">
         <v>1458</v>
       </c>
       <c r="BQ43" s="358" t="s">
@@ -39046,12 +39018,12 @@
       <c r="BV43" s="278" t="s">
         <v>1455</v>
       </c>
-      <c r="BW43" s="790"/>
+      <c r="BW43" s="789"/>
     </row>
-    <row r="44" spans="1:75" s="773" customFormat="1" ht="45" customHeight="1">
+    <row r="44" spans="1:75" s="772" customFormat="1" ht="45" customHeight="1">
       <c r="A44" s="205"/>
-      <c r="B44" s="873"/>
-      <c r="C44" s="789" t="s">
+      <c r="B44" s="872"/>
+      <c r="C44" s="788" t="s">
         <v>1454</v>
       </c>
       <c r="D44" s="263" t="s">
@@ -39146,39 +39118,39 @@
       <c r="AW44" s="119"/>
       <c r="AX44" s="119"/>
       <c r="AY44" s="132"/>
-      <c r="AZ44" s="878" t="s">
+      <c r="AZ44" s="877" t="s">
         <v>1440</v>
       </c>
-      <c r="BA44" s="879"/>
-      <c r="BB44" s="879"/>
-      <c r="BC44" s="879"/>
-      <c r="BD44" s="879"/>
-      <c r="BE44" s="879"/>
-      <c r="BF44" s="879"/>
-      <c r="BG44" s="879"/>
-      <c r="BH44" s="880"/>
-      <c r="BI44" s="788" t="s">
+      <c r="BA44" s="878"/>
+      <c r="BB44" s="878"/>
+      <c r="BC44" s="878"/>
+      <c r="BD44" s="878"/>
+      <c r="BE44" s="878"/>
+      <c r="BF44" s="878"/>
+      <c r="BG44" s="878"/>
+      <c r="BH44" s="879"/>
+      <c r="BI44" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BJ44" s="788" t="s">
+      <c r="BJ44" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BK44" s="788" t="s">
+      <c r="BK44" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BL44" s="788" t="s">
+      <c r="BL44" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BM44" s="788" t="s">
+      <c r="BM44" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BN44" s="788" t="s">
+      <c r="BN44" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BO44" s="788" t="s">
+      <c r="BO44" s="787" t="s">
         <v>1439</v>
       </c>
-      <c r="BP44" s="787" t="s">
+      <c r="BP44" s="786" t="s">
         <v>1439</v>
       </c>
       <c r="BQ44" s="358" t="s">
@@ -39199,9 +39171,9 @@
       </c>
       <c r="BW44" s="167"/>
     </row>
-    <row r="45" spans="1:75" s="773" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A45" s="777"/>
-      <c r="B45" s="874"/>
+    <row r="45" spans="1:75" s="772" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A45" s="776"/>
+      <c r="B45" s="873"/>
       <c r="C45" s="315" t="s">
         <v>1381</v>
       </c>
@@ -39297,7 +39269,7 @@
         <f>L45</f>
         <v>신소재 205</v>
       </c>
-      <c r="AS45" s="786" t="s">
+      <c r="AS45" s="785" t="s">
         <v>1429</v>
       </c>
       <c r="AT45" s="135"/>
@@ -39306,39 +39278,39 @@
       <c r="AW45" s="135"/>
       <c r="AX45" s="135"/>
       <c r="AY45" s="136"/>
-      <c r="AZ45" s="881" t="s">
+      <c r="AZ45" s="880" t="s">
         <v>1428</v>
       </c>
-      <c r="BA45" s="882"/>
-      <c r="BB45" s="882"/>
-      <c r="BC45" s="882"/>
-      <c r="BD45" s="882"/>
-      <c r="BE45" s="882"/>
-      <c r="BF45" s="882"/>
-      <c r="BG45" s="882"/>
-      <c r="BH45" s="883"/>
-      <c r="BI45" s="785" t="s">
+      <c r="BA45" s="881"/>
+      <c r="BB45" s="881"/>
+      <c r="BC45" s="881"/>
+      <c r="BD45" s="881"/>
+      <c r="BE45" s="881"/>
+      <c r="BF45" s="881"/>
+      <c r="BG45" s="881"/>
+      <c r="BH45" s="882"/>
+      <c r="BI45" s="784" t="s">
         <v>1427</v>
       </c>
-      <c r="BJ45" s="785" t="s">
+      <c r="BJ45" s="784" t="s">
         <v>1426</v>
       </c>
-      <c r="BK45" s="784" t="s">
+      <c r="BK45" s="783" t="s">
         <v>1425</v>
       </c>
-      <c r="BL45" s="784" t="s">
+      <c r="BL45" s="783" t="s">
         <v>1217</v>
       </c>
-      <c r="BM45" s="784" t="s">
+      <c r="BM45" s="783" t="s">
         <v>1424</v>
       </c>
-      <c r="BN45" s="784" t="s">
+      <c r="BN45" s="783" t="s">
         <v>1334</v>
       </c>
-      <c r="BO45" s="784" t="s">
+      <c r="BO45" s="783" t="s">
         <v>1423</v>
       </c>
-      <c r="BP45" s="783" t="s">
+      <c r="BP45" s="782" t="s">
         <v>1211</v>
       </c>
       <c r="BQ45" s="359" t="str">
@@ -39365,10 +39337,10 @@
     </row>
     <row r="46" spans="1:75" s="203" customFormat="1" ht="13.5" customHeight="1">
       <c r="A46" s="202"/>
-      <c r="B46" s="887" t="s">
+      <c r="B46" s="886" t="s">
         <v>1421</v>
       </c>
-      <c r="C46" s="772" t="s">
+      <c r="C46" s="771" t="s">
         <v>1311</v>
       </c>
       <c r="D46" s="189" t="s">
@@ -39382,7 +39354,7 @@
       </c>
       <c r="G46" s="112"/>
       <c r="H46" s="114"/>
-      <c r="I46" s="782"/>
+      <c r="I46" s="781"/>
       <c r="J46" s="228" t="s">
         <v>1419</v>
       </c>
@@ -39397,13 +39369,13 @@
       <c r="Q46" s="156"/>
       <c r="R46" s="156"/>
       <c r="S46" s="141"/>
-      <c r="T46" s="771" t="s">
+      <c r="T46" s="770" t="s">
         <v>815</v>
       </c>
       <c r="U46" s="112" t="s">
         <v>1417</v>
       </c>
-      <c r="V46" s="781" t="s">
+      <c r="V46" s="780" t="s">
         <v>199</v>
       </c>
       <c r="W46" s="112"/>
@@ -39465,10 +39437,10 @@
       <c r="BC46" s="126"/>
       <c r="BD46" s="126"/>
       <c r="BE46" s="126"/>
-      <c r="BF46" s="780" t="s">
+      <c r="BF46" s="779" t="s">
         <v>693</v>
       </c>
-      <c r="BG46" s="779" t="s">
+      <c r="BG46" s="778" t="s">
         <v>1407</v>
       </c>
       <c r="BH46" s="126"/>
@@ -39492,8 +39464,8 @@
     </row>
     <row r="47" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A47" s="205"/>
-      <c r="B47" s="888"/>
-      <c r="C47" s="769" t="s">
+      <c r="B47" s="887"/>
+      <c r="C47" s="768" t="s">
         <v>0</v>
       </c>
       <c r="D47" s="149" t="s">
@@ -39528,7 +39500,7 @@
       <c r="U47" s="120" t="s">
         <v>2038</v>
       </c>
-      <c r="V47" s="778" t="s">
+      <c r="V47" s="777" t="s">
         <v>1403</v>
       </c>
       <c r="W47" s="120"/>
@@ -39617,8 +39589,8 @@
     </row>
     <row r="48" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A48" s="205"/>
-      <c r="B48" s="888"/>
-      <c r="C48" s="769" t="s">
+      <c r="B48" s="887"/>
+      <c r="C48" s="768" t="s">
         <v>1</v>
       </c>
       <c r="D48" s="320" t="s">
@@ -39653,7 +39625,7 @@
       <c r="U48" s="120" t="s">
         <v>1395</v>
       </c>
-      <c r="V48" s="778" t="s">
+      <c r="V48" s="777" t="s">
         <v>1394</v>
       </c>
       <c r="W48" s="120"/>
@@ -39740,9 +39712,9 @@
       <c r="BV48" s="119"/>
       <c r="BW48" s="159"/>
     </row>
-    <row r="49" spans="1:75" s="773" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A49" s="777"/>
-      <c r="B49" s="889"/>
+    <row r="49" spans="1:75" s="772" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A49" s="776"/>
+      <c r="B49" s="888"/>
       <c r="C49" s="164" t="s">
         <v>1381</v>
       </c>
@@ -39772,13 +39744,13 @@
       <c r="Q49" s="136"/>
       <c r="R49" s="136"/>
       <c r="S49" s="137"/>
-      <c r="T49" s="776" t="s">
+      <c r="T49" s="775" t="s">
         <v>1341</v>
       </c>
       <c r="U49" s="134" t="s">
         <v>1334</v>
       </c>
-      <c r="V49" s="775" t="s">
+      <c r="V49" s="774" t="s">
         <v>1340</v>
       </c>
       <c r="W49" s="134"/>
@@ -39799,7 +39771,7 @@
       <c r="AG49" s="145"/>
       <c r="AH49" s="145"/>
       <c r="AI49" s="145"/>
-      <c r="AJ49" s="852" t="s">
+      <c r="AJ49" s="851" t="s">
         <v>2043</v>
       </c>
       <c r="AK49" s="135" t="s">
@@ -39814,24 +39786,24 @@
       <c r="AN49" s="135" t="s">
         <v>1335</v>
       </c>
-      <c r="AO49" s="855" t="s">
+      <c r="AO49" s="854" t="s">
         <v>2047</v>
       </c>
-      <c r="AP49" s="774" t="str">
+      <c r="AP49" s="773" t="str">
         <f>AO41</f>
         <v>대학A 229</v>
       </c>
       <c r="AQ49" s="135" t="s">
         <v>1342</v>
       </c>
-      <c r="AR49" s="766"/>
-      <c r="AS49" s="766"/>
-      <c r="AT49" s="766"/>
-      <c r="AU49" s="766"/>
-      <c r="AV49" s="767"/>
-      <c r="AW49" s="767"/>
-      <c r="AX49" s="767"/>
-      <c r="AY49" s="767"/>
+      <c r="AR49" s="765"/>
+      <c r="AS49" s="765"/>
+      <c r="AT49" s="765"/>
+      <c r="AU49" s="765"/>
+      <c r="AV49" s="766"/>
+      <c r="AW49" s="766"/>
+      <c r="AX49" s="766"/>
+      <c r="AY49" s="766"/>
       <c r="AZ49" s="139" t="s">
         <v>1334</v>
       </c>
@@ -39849,15 +39821,15 @@
         <f>BG37</f>
         <v>대학B 115</v>
       </c>
-      <c r="BH49" s="766"/>
-      <c r="BI49" s="766"/>
-      <c r="BJ49" s="766"/>
-      <c r="BK49" s="766"/>
-      <c r="BL49" s="765"/>
-      <c r="BM49" s="765"/>
-      <c r="BN49" s="765"/>
-      <c r="BO49" s="765"/>
-      <c r="BP49" s="765"/>
+      <c r="BH49" s="765"/>
+      <c r="BI49" s="765"/>
+      <c r="BJ49" s="765"/>
+      <c r="BK49" s="765"/>
+      <c r="BL49" s="764"/>
+      <c r="BM49" s="764"/>
+      <c r="BN49" s="764"/>
+      <c r="BO49" s="764"/>
+      <c r="BP49" s="764"/>
       <c r="BQ49" s="150"/>
       <c r="BR49" s="134"/>
       <c r="BS49" s="135"/>
@@ -39867,14 +39839,14 @@
       </c>
       <c r="BU49" s="188"/>
       <c r="BV49" s="135"/>
-      <c r="BW49" s="744"/>
+      <c r="BW49" s="743"/>
     </row>
     <row r="50" spans="1:75" s="203" customFormat="1" ht="17.25" customHeight="1">
       <c r="A50" s="204"/>
-      <c r="B50" s="890" t="s">
+      <c r="B50" s="889" t="s">
         <v>502</v>
       </c>
-      <c r="C50" s="772" t="s">
+      <c r="C50" s="771" t="s">
         <v>1311</v>
       </c>
       <c r="D50" s="189" t="s">
@@ -39903,13 +39875,13 @@
       <c r="Q50" s="372"/>
       <c r="R50" s="372"/>
       <c r="S50" s="171"/>
-      <c r="T50" s="771" t="s">
+      <c r="T50" s="770" t="s">
         <v>815</v>
       </c>
       <c r="U50" s="113" t="s">
         <v>1094</v>
       </c>
-      <c r="V50" s="771" t="s">
+      <c r="V50" s="770" t="s">
         <v>815</v>
       </c>
       <c r="W50" s="120" t="s">
@@ -39938,7 +39910,7 @@
       <c r="AL50" s="156" t="s">
         <v>1369</v>
       </c>
-      <c r="AM50" s="856" t="s">
+      <c r="AM50" s="855" t="s">
         <v>2049</v>
       </c>
       <c r="AN50" s="112"/>
@@ -39953,7 +39925,7 @@
       <c r="AW50" s="113"/>
       <c r="AX50" s="113"/>
       <c r="AY50" s="113"/>
-      <c r="AZ50" s="770" t="s">
+      <c r="AZ50" s="769" t="s">
         <v>1368</v>
       </c>
       <c r="BA50" s="126"/>
@@ -39984,8 +39956,8 @@
     </row>
     <row r="51" spans="1:75" s="203" customFormat="1" ht="23.1" customHeight="1">
       <c r="A51" s="204"/>
-      <c r="B51" s="891"/>
-      <c r="C51" s="769" t="s">
+      <c r="B51" s="890"/>
+      <c r="C51" s="768" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="149" t="s">
@@ -40095,8 +40067,8 @@
     </row>
     <row r="52" spans="1:75" s="203" customFormat="1" ht="45" customHeight="1">
       <c r="A52" s="204"/>
-      <c r="B52" s="891"/>
-      <c r="C52" s="769" t="s">
+      <c r="B52" s="890"/>
+      <c r="C52" s="768" t="s">
         <v>1</v>
       </c>
       <c r="D52" s="320" t="s">
@@ -40206,7 +40178,7 @@
     </row>
     <row r="53" spans="1:75" s="181" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
       <c r="A53" s="182"/>
-      <c r="B53" s="892"/>
+      <c r="B53" s="891"/>
       <c r="C53" s="191" t="s">
         <v>500</v>
       </c>
@@ -40236,7 +40208,7 @@
       <c r="Q53" s="164"/>
       <c r="R53" s="164"/>
       <c r="S53" s="138"/>
-      <c r="T53" s="768" t="s">
+      <c r="T53" s="767" t="s">
         <v>1341</v>
       </c>
       <c r="U53" s="145" t="s">
@@ -40262,7 +40234,7 @@
       <c r="AG53" s="136"/>
       <c r="AH53" s="136"/>
       <c r="AI53" s="136"/>
-      <c r="AJ53" s="853" t="s">
+      <c r="AJ53" s="852" t="s">
         <v>2042</v>
       </c>
       <c r="AK53" s="134" t="s">
@@ -40271,43 +40243,43 @@
       <c r="AL53" s="136" t="s">
         <v>1335</v>
       </c>
-      <c r="AM53" s="849" t="s">
+      <c r="AM53" s="848" t="s">
         <v>2027</v>
       </c>
-      <c r="AN53" s="766"/>
-      <c r="AO53" s="766"/>
-      <c r="AP53" s="766"/>
-      <c r="AQ53" s="766"/>
-      <c r="AR53" s="766"/>
-      <c r="AS53" s="766"/>
-      <c r="AT53" s="766"/>
-      <c r="AU53" s="766"/>
-      <c r="AV53" s="767"/>
-      <c r="AW53" s="767"/>
-      <c r="AX53" s="767"/>
-      <c r="AY53" s="767"/>
+      <c r="AN53" s="765"/>
+      <c r="AO53" s="765"/>
+      <c r="AP53" s="765"/>
+      <c r="AQ53" s="765"/>
+      <c r="AR53" s="765"/>
+      <c r="AS53" s="765"/>
+      <c r="AT53" s="765"/>
+      <c r="AU53" s="765"/>
+      <c r="AV53" s="766"/>
+      <c r="AW53" s="766"/>
+      <c r="AX53" s="766"/>
+      <c r="AY53" s="766"/>
       <c r="AZ53" s="139" t="s">
         <v>1334</v>
       </c>
       <c r="BA53" s="134"/>
       <c r="BB53" s="134"/>
-      <c r="BC53" s="766"/>
-      <c r="BD53" s="766"/>
-      <c r="BE53" s="766"/>
-      <c r="BF53" s="766"/>
+      <c r="BC53" s="765"/>
+      <c r="BD53" s="765"/>
+      <c r="BE53" s="765"/>
+      <c r="BF53" s="765"/>
       <c r="BG53" s="279" t="str">
         <f>BG49</f>
         <v>대학B 115</v>
       </c>
-      <c r="BH53" s="766"/>
-      <c r="BI53" s="766"/>
-      <c r="BJ53" s="766"/>
-      <c r="BK53" s="766"/>
-      <c r="BL53" s="765"/>
-      <c r="BM53" s="765"/>
-      <c r="BN53" s="765"/>
-      <c r="BO53" s="765"/>
-      <c r="BP53" s="765"/>
+      <c r="BH53" s="765"/>
+      <c r="BI53" s="765"/>
+      <c r="BJ53" s="765"/>
+      <c r="BK53" s="765"/>
+      <c r="BL53" s="764"/>
+      <c r="BM53" s="764"/>
+      <c r="BN53" s="764"/>
+      <c r="BO53" s="764"/>
+      <c r="BP53" s="764"/>
       <c r="BQ53" s="150"/>
       <c r="BR53" s="134"/>
       <c r="BS53" s="75"/>
@@ -40319,7 +40291,7 @@
     <row r="54" spans="1:75" s="73" customFormat="1" ht="14.25" thickBot="1">
       <c r="A54" s="322"/>
       <c r="B54" s="15"/>
-      <c r="C54" s="764"/>
+      <c r="C54" s="763"/>
       <c r="D54" s="165"/>
       <c r="E54" s="165"/>
       <c r="F54" s="165"/>
@@ -40395,10 +40367,10 @@
     </row>
     <row r="55" spans="1:75" s="181" customFormat="1" ht="15" customHeight="1">
       <c r="A55" s="180"/>
-      <c r="B55" s="866" t="s">
+      <c r="B55" s="865" t="s">
         <v>509</v>
       </c>
-      <c r="C55" s="753" t="s">
+      <c r="C55" s="752" t="s">
         <v>1311</v>
       </c>
       <c r="D55" s="189" t="s">
@@ -40463,7 +40435,7 @@
       <c r="AW55" s="116"/>
       <c r="AX55" s="116"/>
       <c r="AY55" s="117"/>
-      <c r="AZ55" s="763" t="s">
+      <c r="AZ55" s="762" t="s">
         <v>1327</v>
       </c>
       <c r="BA55" s="415" t="s">
@@ -40482,7 +40454,7 @@
       <c r="BL55" s="166"/>
       <c r="BM55" s="166"/>
       <c r="BN55" s="166"/>
-      <c r="BO55" s="762"/>
+      <c r="BO55" s="761"/>
       <c r="BP55" s="199"/>
       <c r="BQ55" s="739" t="s">
         <v>724</v>
@@ -40502,11 +40474,11 @@
     </row>
     <row r="56" spans="1:75" s="181" customFormat="1" ht="23.1" customHeight="1">
       <c r="A56" s="6"/>
-      <c r="B56" s="867"/>
-      <c r="C56" s="752" t="s">
+      <c r="B56" s="866"/>
+      <c r="C56" s="751" t="s">
         <v>0</v>
       </c>
-      <c r="D56" s="854" t="s">
+      <c r="D56" s="853" t="s">
         <v>2044</v>
       </c>
       <c r="E56" s="131" t="s">
@@ -40526,7 +40498,7 @@
       <c r="Q56" s="131"/>
       <c r="R56" s="131"/>
       <c r="S56" s="131"/>
-      <c r="T56" s="854" t="s">
+      <c r="T56" s="853" t="s">
         <v>2044</v>
       </c>
       <c r="U56" s="131" t="s">
@@ -40548,7 +40520,7 @@
       <c r="AG56" s="131"/>
       <c r="AH56" s="131"/>
       <c r="AI56" s="163"/>
-      <c r="AJ56" s="854" t="s">
+      <c r="AJ56" s="853" t="s">
         <v>2046</v>
       </c>
       <c r="AK56" s="131" t="s">
@@ -40568,7 +40540,7 @@
       <c r="AW56" s="131"/>
       <c r="AX56" s="131"/>
       <c r="AY56" s="167"/>
-      <c r="AZ56" s="757" t="s">
+      <c r="AZ56" s="756" t="s">
         <v>508</v>
       </c>
       <c r="BA56" s="131" t="s">
@@ -40587,7 +40559,7 @@
       <c r="BL56" s="168"/>
       <c r="BM56" s="168"/>
       <c r="BN56" s="168"/>
-      <c r="BO56" s="758"/>
+      <c r="BO56" s="757"/>
       <c r="BP56" s="200"/>
       <c r="BQ56" s="740" t="s">
         <v>1322</v>
@@ -40607,8 +40579,8 @@
     </row>
     <row r="57" spans="1:75" s="181" customFormat="1" ht="45" customHeight="1">
       <c r="A57" s="6"/>
-      <c r="B57" s="867"/>
-      <c r="C57" s="752" t="s">
+      <c r="B57" s="866"/>
+      <c r="C57" s="751" t="s">
         <v>1</v>
       </c>
       <c r="D57" s="320" t="s">
@@ -40673,7 +40645,7 @@
       <c r="AW57" s="131"/>
       <c r="AX57" s="131"/>
       <c r="AY57" s="167"/>
-      <c r="AZ57" s="757" t="s">
+      <c r="AZ57" s="756" t="s">
         <v>722</v>
       </c>
       <c r="BA57" s="131" t="s">
@@ -40692,7 +40664,7 @@
       <c r="BL57" s="168"/>
       <c r="BM57" s="168"/>
       <c r="BN57" s="168"/>
-      <c r="BO57" s="758"/>
+      <c r="BO57" s="757"/>
       <c r="BP57" s="200"/>
       <c r="BQ57" s="740" t="s">
         <v>723</v>
@@ -40712,7 +40684,7 @@
     </row>
     <row r="58" spans="1:75" s="181" customFormat="1" ht="18" customHeight="1">
       <c r="A58" s="182"/>
-      <c r="B58" s="893"/>
+      <c r="B58" s="892"/>
       <c r="C58" s="190" t="s">
         <v>1293</v>
       </c>
@@ -40778,7 +40750,7 @@
       <c r="AW58" s="74"/>
       <c r="AX58" s="74"/>
       <c r="AY58" s="169"/>
-      <c r="AZ58" s="761" t="s">
+      <c r="AZ58" s="760" t="s">
         <v>1291</v>
       </c>
       <c r="BA58" s="74" t="s">
@@ -40817,16 +40789,16 @@
     </row>
     <row r="59" spans="1:75" s="181" customFormat="1" ht="15" customHeight="1">
       <c r="A59" s="180"/>
-      <c r="B59" s="894" t="s">
+      <c r="B59" s="893" t="s">
         <v>1312</v>
       </c>
-      <c r="C59" s="760" t="s">
+      <c r="C59" s="759" t="s">
         <v>1311</v>
       </c>
       <c r="D59" s="173" t="s">
         <v>1310</v>
       </c>
-      <c r="E59" s="759" t="s">
+      <c r="E59" s="758" t="s">
         <v>1309</v>
       </c>
       <c r="F59" s="123"/>
@@ -40885,7 +40857,7 @@
       <c r="AW59" s="123"/>
       <c r="AX59" s="123"/>
       <c r="AY59" s="124"/>
-      <c r="AZ59" s="757"/>
+      <c r="AZ59" s="756"/>
       <c r="BA59" s="123"/>
       <c r="BB59" s="123"/>
       <c r="BC59" s="123"/>
@@ -40900,7 +40872,7 @@
       <c r="BL59" s="168"/>
       <c r="BM59" s="168"/>
       <c r="BN59" s="168"/>
-      <c r="BO59" s="758"/>
+      <c r="BO59" s="757"/>
       <c r="BP59" s="200"/>
       <c r="BQ59" s="173" t="s">
         <v>1305</v>
@@ -40916,11 +40888,11 @@
     </row>
     <row r="60" spans="1:75" s="181" customFormat="1" ht="23.1" customHeight="1">
       <c r="A60" s="6"/>
-      <c r="B60" s="870"/>
-      <c r="C60" s="752" t="s">
+      <c r="B60" s="869"/>
+      <c r="C60" s="751" t="s">
         <v>0</v>
       </c>
-      <c r="D60" s="854" t="s">
+      <c r="D60" s="853" t="s">
         <v>2044</v>
       </c>
       <c r="E60" s="131" t="s">
@@ -40940,7 +40912,7 @@
       <c r="Q60" s="131"/>
       <c r="R60" s="131"/>
       <c r="S60" s="131"/>
-      <c r="T60" s="854" t="s">
+      <c r="T60" s="853" t="s">
         <v>2045</v>
       </c>
       <c r="U60" s="131" t="s">
@@ -40962,7 +40934,7 @@
       <c r="AG60" s="131"/>
       <c r="AH60" s="131"/>
       <c r="AI60" s="163"/>
-      <c r="AJ60" s="854" t="s">
+      <c r="AJ60" s="853" t="s">
         <v>2046</v>
       </c>
       <c r="AK60" s="131" t="s">
@@ -40982,7 +40954,7 @@
       <c r="AW60" s="131"/>
       <c r="AX60" s="131"/>
       <c r="AY60" s="167"/>
-      <c r="AZ60" s="757"/>
+      <c r="AZ60" s="756"/>
       <c r="BA60" s="131"/>
       <c r="BB60" s="131"/>
       <c r="BC60" s="131"/>
@@ -40997,7 +40969,7 @@
       <c r="BL60" s="172"/>
       <c r="BM60" s="172"/>
       <c r="BN60" s="172"/>
-      <c r="BO60" s="756"/>
+      <c r="BO60" s="755"/>
       <c r="BP60" s="201"/>
       <c r="BQ60" s="149" t="s">
         <v>508</v>
@@ -41013,8 +40985,8 @@
     </row>
     <row r="61" spans="1:75" s="181" customFormat="1" ht="45" customHeight="1">
       <c r="A61" s="6"/>
-      <c r="B61" s="870"/>
-      <c r="C61" s="752" t="s">
+      <c r="B61" s="869"/>
+      <c r="C61" s="751" t="s">
         <v>1</v>
       </c>
       <c r="D61" s="149" t="s">
@@ -41079,7 +41051,7 @@
       <c r="AW61" s="131"/>
       <c r="AX61" s="131"/>
       <c r="AY61" s="167"/>
-      <c r="AZ61" s="757"/>
+      <c r="AZ61" s="756"/>
       <c r="BA61" s="131"/>
       <c r="BB61" s="131"/>
       <c r="BC61" s="131"/>
@@ -41094,7 +41066,7 @@
       <c r="BL61" s="172"/>
       <c r="BM61" s="172"/>
       <c r="BN61" s="172"/>
-      <c r="BO61" s="756"/>
+      <c r="BO61" s="755"/>
       <c r="BP61" s="201"/>
       <c r="BQ61" s="149" t="s">
         <v>1295</v>
@@ -41110,7 +41082,7 @@
     </row>
     <row r="62" spans="1:75" s="181" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A62" s="182"/>
-      <c r="B62" s="871"/>
+      <c r="B62" s="870"/>
       <c r="C62" s="191" t="s">
         <v>1293</v>
       </c>
@@ -41176,7 +41148,7 @@
       <c r="AW62" s="75"/>
       <c r="AX62" s="75"/>
       <c r="AY62" s="138"/>
-      <c r="AZ62" s="755"/>
+      <c r="AZ62" s="754"/>
       <c r="BA62" s="75"/>
       <c r="BB62" s="75"/>
       <c r="BC62" s="75"/>
@@ -41208,7 +41180,7 @@
     <row r="63" spans="1:75" ht="14.25" thickBot="1">
       <c r="A63" s="322"/>
       <c r="B63" s="322"/>
-      <c r="C63" s="754"/>
+      <c r="C63" s="753"/>
       <c r="D63" s="322"/>
       <c r="E63" s="322"/>
       <c r="F63" s="322"/>
@@ -41283,10 +41255,10 @@
     </row>
     <row r="64" spans="1:75" ht="13.5">
       <c r="A64" s="15"/>
-      <c r="B64" s="869" t="s">
+      <c r="B64" s="868" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="753" t="s">
+      <c r="C64" s="752" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="17"/>
@@ -41368,8 +41340,8 @@
     </row>
     <row r="65" spans="1:75" ht="23.1" customHeight="1">
       <c r="A65" s="15"/>
-      <c r="B65" s="870"/>
-      <c r="C65" s="752" t="s">
+      <c r="B65" s="869"/>
+      <c r="C65" s="751" t="s">
         <v>0</v>
       </c>
       <c r="D65" s="26"/>
@@ -41451,8 +41423,8 @@
     </row>
     <row r="66" spans="1:75" ht="45" customHeight="1">
       <c r="A66" s="15"/>
-      <c r="B66" s="870"/>
-      <c r="C66" s="752" t="s">
+      <c r="B66" s="869"/>
+      <c r="C66" s="751" t="s">
         <v>1</v>
       </c>
       <c r="D66" s="31"/>
@@ -41534,8 +41506,8 @@
     </row>
     <row r="67" spans="1:75" ht="23.1" customHeight="1" thickBot="1">
       <c r="A67" s="15"/>
-      <c r="B67" s="871"/>
-      <c r="C67" s="750" t="s">
+      <c r="B67" s="870"/>
+      <c r="C67" s="749" t="s">
         <v>19</v>
       </c>
       <c r="D67" s="41"/>
@@ -41617,10 +41589,10 @@
     </row>
     <row r="68" spans="1:75" ht="13.5">
       <c r="A68" s="15"/>
-      <c r="B68" s="866" t="s">
+      <c r="B68" s="865" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="753" t="s">
+      <c r="C68" s="752" t="s">
         <v>14</v>
       </c>
       <c r="D68" s="17" t="s">
@@ -41748,8 +41720,8 @@
     </row>
     <row r="69" spans="1:75" ht="23.1" customHeight="1">
       <c r="A69" s="15"/>
-      <c r="B69" s="867"/>
-      <c r="C69" s="752" t="s">
+      <c r="B69" s="866"/>
+      <c r="C69" s="751" t="s">
         <v>0</v>
       </c>
       <c r="D69" s="26" t="s">
@@ -41863,7 +41835,7 @@
       <c r="BL69" s="29"/>
       <c r="BM69" s="29"/>
       <c r="BN69" s="48"/>
-      <c r="BO69" s="751"/>
+      <c r="BO69" s="750"/>
       <c r="BP69" s="49"/>
       <c r="BQ69" s="26" t="s">
         <v>1185</v>
@@ -41877,8 +41849,8 @@
     </row>
     <row r="70" spans="1:75" ht="45" customHeight="1">
       <c r="A70" s="15"/>
-      <c r="B70" s="867"/>
-      <c r="C70" s="752" t="s">
+      <c r="B70" s="866"/>
+      <c r="C70" s="751" t="s">
         <v>1</v>
       </c>
       <c r="D70" s="31" t="s">
@@ -41992,7 +41964,7 @@
       <c r="BL70" s="29"/>
       <c r="BM70" s="29"/>
       <c r="BN70" s="48"/>
-      <c r="BO70" s="751"/>
+      <c r="BO70" s="750"/>
       <c r="BP70" s="49"/>
       <c r="BQ70" s="31" t="s">
         <v>43</v>
@@ -42006,8 +41978,8 @@
     </row>
     <row r="71" spans="1:75" ht="23.1" customHeight="1" thickBot="1">
       <c r="A71" s="15"/>
-      <c r="B71" s="868"/>
-      <c r="C71" s="750" t="s">
+      <c r="B71" s="867"/>
+      <c r="C71" s="749" t="s">
         <v>19</v>
       </c>
       <c r="D71" s="41" t="s">
@@ -42121,7 +42093,7 @@
       <c r="BL71" s="52"/>
       <c r="BM71" s="52"/>
       <c r="BN71" s="53"/>
-      <c r="BO71" s="749"/>
+      <c r="BO71" s="748"/>
       <c r="BP71" s="55"/>
       <c r="BQ71" s="64" t="s">
         <v>1257</v>
@@ -42135,10 +42107,10 @@
     </row>
     <row r="72" spans="1:75" ht="13.5" customHeight="1">
       <c r="A72" s="15"/>
-      <c r="B72" s="867" t="s">
+      <c r="B72" s="866" t="s">
         <v>59</v>
       </c>
-      <c r="C72" s="748" t="s">
+      <c r="C72" s="747" t="s">
         <v>14</v>
       </c>
       <c r="D72" s="58" t="s">
@@ -42272,8 +42244,8 @@
     </row>
     <row r="73" spans="1:75" ht="23.1" customHeight="1">
       <c r="A73" s="15"/>
-      <c r="B73" s="867"/>
-      <c r="C73" s="747" t="s">
+      <c r="B73" s="866"/>
+      <c r="C73" s="746" t="s">
         <v>0</v>
       </c>
       <c r="D73" s="26" t="s">
@@ -42407,8 +42379,8 @@
     </row>
     <row r="74" spans="1:75" ht="45" customHeight="1">
       <c r="A74" s="15"/>
-      <c r="B74" s="867"/>
-      <c r="C74" s="747" t="s">
+      <c r="B74" s="866"/>
+      <c r="C74" s="746" t="s">
         <v>1</v>
       </c>
       <c r="D74" s="31" t="s">
@@ -42542,8 +42514,8 @@
     </row>
     <row r="75" spans="1:75" ht="23.1" customHeight="1" thickBot="1">
       <c r="A75" s="15"/>
-      <c r="B75" s="868"/>
-      <c r="C75" s="746" t="s">
+      <c r="B75" s="867"/>
+      <c r="C75" s="745" t="s">
         <v>19</v>
       </c>
       <c r="D75" s="41" t="s">
@@ -42817,12 +42789,12 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D4:O4"/>
     <mergeCell ref="AJ4:AY4"/>
     <mergeCell ref="T4:AI4"/>
     <mergeCell ref="AZ4:BP4"/>
     <mergeCell ref="B30:B37"/>
     <mergeCell ref="AZ42:BH42"/>
+    <mergeCell ref="D4:S4"/>
     <mergeCell ref="BQ4:BW4"/>
     <mergeCell ref="B72:B75"/>
     <mergeCell ref="B46:B49"/>
@@ -43184,21 +43156,21 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="51" customHeight="1">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>979</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
     </row>
     <row r="3" spans="1:13" ht="8.25" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:13" ht="42" customHeight="1">
@@ -43739,23 +43711,23 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="26.25">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>979</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
-      <c r="N2" s="858"/>
-      <c r="O2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
+      <c r="N2" s="857"/>
+      <c r="O2" s="857"/>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:15" ht="43.5" customHeight="1">
@@ -44370,23 +44342,23 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="26.25">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>979</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
-      <c r="N2" s="858"/>
-      <c r="O2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
+      <c r="N2" s="857"/>
+      <c r="O2" s="857"/>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:15" ht="43.5" customHeight="1" thickBot="1">
@@ -44977,23 +44949,23 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="26.25">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>979</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
-      <c r="N2" s="858"/>
-      <c r="O2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
+      <c r="N2" s="857"/>
+      <c r="O2" s="857"/>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:15" ht="43.5" customHeight="1" thickBot="1">
@@ -45715,22 +45687,22 @@
   <sheetData>
     <row r="1" spans="1:15" ht="36.75" customHeight="1">
       <c r="A1" s="8"/>
-      <c r="B1" s="858" t="s">
+      <c r="B1" s="857" t="s">
         <v>979</v>
       </c>
-      <c r="C1" s="858"/>
-      <c r="D1" s="858"/>
-      <c r="E1" s="858"/>
-      <c r="F1" s="858"/>
-      <c r="G1" s="858"/>
-      <c r="H1" s="858"/>
-      <c r="I1" s="858"/>
-      <c r="J1" s="858"/>
-      <c r="K1" s="858"/>
-      <c r="L1" s="858"/>
-      <c r="M1" s="858"/>
-      <c r="N1" s="858"/>
-      <c r="O1" s="858"/>
+      <c r="C1" s="857"/>
+      <c r="D1" s="857"/>
+      <c r="E1" s="857"/>
+      <c r="F1" s="857"/>
+      <c r="G1" s="857"/>
+      <c r="H1" s="857"/>
+      <c r="I1" s="857"/>
+      <c r="J1" s="857"/>
+      <c r="K1" s="857"/>
+      <c r="L1" s="857"/>
+      <c r="M1" s="857"/>
+      <c r="N1" s="857"/>
+      <c r="O1" s="857"/>
     </row>
     <row r="2" spans="1:15" ht="17.25" thickBot="1">
       <c r="A2" s="531"/>
@@ -46588,23 +46560,23 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="26.25">
-      <c r="A2" s="858" t="s">
+      <c r="A2" s="857" t="s">
         <v>979</v>
       </c>
-      <c r="B2" s="858"/>
-      <c r="C2" s="858"/>
-      <c r="D2" s="858"/>
-      <c r="E2" s="858"/>
-      <c r="F2" s="858"/>
-      <c r="G2" s="858"/>
-      <c r="H2" s="858"/>
-      <c r="I2" s="858"/>
-      <c r="J2" s="858"/>
-      <c r="K2" s="858"/>
-      <c r="L2" s="858"/>
-      <c r="M2" s="858"/>
-      <c r="N2" s="858"/>
-      <c r="O2" s="858"/>
+      <c r="B2" s="857"/>
+      <c r="C2" s="857"/>
+      <c r="D2" s="857"/>
+      <c r="E2" s="857"/>
+      <c r="F2" s="857"/>
+      <c r="G2" s="857"/>
+      <c r="H2" s="857"/>
+      <c r="I2" s="857"/>
+      <c r="J2" s="857"/>
+      <c r="K2" s="857"/>
+      <c r="L2" s="857"/>
+      <c r="M2" s="857"/>
+      <c r="N2" s="857"/>
+      <c r="O2" s="857"/>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:15" ht="43.5" customHeight="1" thickBot="1">

</xml_diff>